<commit_message>
DeepLearning --- DONEgit add .git add .git add .
</commit_message>
<xml_diff>
--- a/Times&Accuracy.xlsx
+++ b/Times&Accuracy.xlsx
@@ -32,9 +32,6 @@
     <t>Algorithm</t>
   </si>
   <si>
-    <t>32.366209s</t>
-  </si>
-  <si>
     <t>random forest</t>
   </si>
   <si>
@@ -57,6 +54,9 @@
   </si>
   <si>
     <t>13.424952s</t>
+  </si>
+  <si>
+    <t>28.95758s</t>
   </si>
 </sst>
 </file>
@@ -394,7 +394,7 @@
   <dimension ref="A1:I6"/>
   <sheetViews>
     <sheetView rightToLeft="1" tabSelected="1" workbookViewId="0">
-      <selection activeCell="G8" sqref="G8"/>
+      <selection activeCell="C6" sqref="A1:C6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
@@ -412,23 +412,26 @@
         <v>0</v>
       </c>
       <c r="C1" s="3" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
     </row>
     <row r="2" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A2" s="2" t="s">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="B2" s="2" t="s">
-        <v>2</v>
+        <v>10</v>
+      </c>
+      <c r="C2" s="2">
+        <v>0.95679000000000003</v>
       </c>
     </row>
     <row r="3" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A3" s="2" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="B3" s="2" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="C3" s="2">
         <v>0.92589999999999995</v>
@@ -436,10 +439,10 @@
     </row>
     <row r="4" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A4" s="2" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="B4" s="2" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="C4" s="2">
         <v>0.96699999999999997</v>
@@ -447,10 +450,13 @@
     </row>
     <row r="5" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A5" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="B5" s="2" t="s">
         <v>9</v>
       </c>
-      <c r="B5" s="2" t="s">
-        <v>10</v>
+      <c r="C5" s="2">
+        <v>0.96</v>
       </c>
     </row>
     <row r="6" spans="1:9" x14ac:dyDescent="0.2">

</xml_diff>

<commit_message>
update Time $ Accuracy
</commit_message>
<xml_diff>
--- a/Times&Accuracy.xlsx
+++ b/Times&Accuracy.xlsx
@@ -1,15 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
-  <workbookPr defaultThemeVersion="153222"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="19330"/>
+  <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\RENT\Desktop\Satellite-communication\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\ספיר יהודה\Satellite-communication\"/>
     </mc:Choice>
   </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{31939276-6FF7-4EF1-AEF8-DE4014CBAE2C}" xr6:coauthVersionLast="33" xr6:coauthVersionMax="33" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="20490" windowHeight="7755"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="20490" windowHeight="7760" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -32,38 +33,38 @@
     <t>Algorithm</t>
   </si>
   <si>
-    <t>random forest</t>
-  </si>
-  <si>
-    <t>svm</t>
-  </si>
-  <si>
-    <t>adaBoost</t>
-  </si>
-  <si>
-    <t>52.892143s</t>
-  </si>
-  <si>
     <t>Accuracy</t>
   </si>
   <si>
-    <t>6.031668s</t>
-  </si>
-  <si>
     <t>Deep Learning</t>
   </si>
   <si>
-    <t>13.424952s</t>
-  </si>
-  <si>
-    <t>28.95758s</t>
+    <t>Random Forest</t>
+  </si>
+  <si>
+    <t>6.558833s</t>
+  </si>
+  <si>
+    <t>SVM</t>
+  </si>
+  <si>
+    <t>5.836301s</t>
+  </si>
+  <si>
+    <t>AdaBoost</t>
+  </si>
+  <si>
+    <t>5.571954s</t>
+  </si>
+  <si>
+    <t>5.430689s</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="2" x14ac:knownFonts="1">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+  <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -74,21 +75,32 @@
     <font>
       <b/>
       <sz val="11"/>
-      <color theme="1"/>
+      <color rgb="FF000000"/>
       <name val="Arial"/>
       <family val="2"/>
-      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF000000"/>
+      <name val="Arial"/>
+      <family val="2"/>
     </font>
   </fonts>
-  <fills count="2">
+  <fills count="3">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFFFF"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="1">
+  <borders count="2">
     <border>
       <left/>
       <right/>
@@ -96,11 +108,26 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="4">
+  <cellXfs count="5">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="right"/>
@@ -108,8 +135,11 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center"/>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" readingOrder="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" readingOrder="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -390,21 +420,21 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:I6"/>
   <sheetViews>
     <sheetView rightToLeft="1" tabSelected="1" workbookViewId="0">
-      <selection activeCell="C6" sqref="A1:C6"/>
+      <selection activeCell="B7" sqref="B7"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultRowHeight="14" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="1" max="1" width="17.75" style="2" customWidth="1"/>
     <col min="2" max="2" width="11.75" style="2" customWidth="1"/>
     <col min="3" max="3" width="10.75" style="2" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9" ht="15" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A1" s="3" t="s">
         <v>1</v>
       </c>
@@ -412,54 +442,54 @@
         <v>0</v>
       </c>
       <c r="C1" s="3" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="2" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A2" s="4" t="s">
+        <v>4</v>
+      </c>
+      <c r="B2" s="4" t="s">
+        <v>5</v>
+      </c>
+      <c r="C2" s="4">
+        <v>0.91395000000000004</v>
+      </c>
+    </row>
+    <row r="3" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A3" s="4" t="s">
         <v>6</v>
       </c>
-    </row>
-    <row r="2" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A2" s="2" t="s">
-        <v>2</v>
-      </c>
-      <c r="B2" s="2" t="s">
+      <c r="B3" s="4" t="s">
+        <v>7</v>
+      </c>
+      <c r="C3" s="4">
+        <v>0.91669999999999996</v>
+      </c>
+    </row>
+    <row r="4" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A4" s="4" t="s">
+        <v>8</v>
+      </c>
+      <c r="B4" s="4" t="s">
+        <v>9</v>
+      </c>
+      <c r="C4" s="4">
+        <v>0.93520000000000003</v>
+      </c>
+    </row>
+    <row r="5" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A5" s="4" t="s">
+        <v>3</v>
+      </c>
+      <c r="B5" s="4" t="s">
         <v>10</v>
       </c>
-      <c r="C2" s="2">
-        <v>0.95679000000000003</v>
-      </c>
-    </row>
-    <row r="3" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A3" s="2" t="s">
-        <v>3</v>
-      </c>
-      <c r="B3" s="2" t="s">
-        <v>5</v>
-      </c>
-      <c r="C3" s="2">
-        <v>0.92589999999999995</v>
-      </c>
-    </row>
-    <row r="4" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A4" s="2" t="s">
-        <v>4</v>
-      </c>
-      <c r="B4" s="2" t="s">
-        <v>7</v>
-      </c>
-      <c r="C4" s="2">
-        <v>0.96699999999999997</v>
-      </c>
-    </row>
-    <row r="5" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A5" s="2" t="s">
-        <v>8</v>
-      </c>
-      <c r="B5" s="2" t="s">
-        <v>9</v>
-      </c>
-      <c r="C5" s="2">
+      <c r="C5" s="4">
         <v>0.96</v>
       </c>
     </row>
-    <row r="6" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:9" x14ac:dyDescent="0.3">
       <c r="I6" s="1"/>
     </row>
   </sheetData>

</xml_diff>